<commit_message>
oaks-crisis: reset xlsx for rerunning for prev months
</commit_message>
<xml_diff>
--- a/src/csv/crisis_sfy_2021.xlsx
+++ b/src/csv/crisis_sfy_2021.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\KHIT\RPA\src\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA2D3CF-FC8D-4C08-AC25-4E1DBFFABFD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D238D01D-DC1C-4E74-B885-7EA4E552C4AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
@@ -696,7 +696,7 @@
   <dimension ref="A1:X75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="K41" sqref="K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>254</v>
+        <v>0</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -869,10 +869,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>522</v>
-      </c>
-      <c r="S3">
-        <v>268</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -892,7 +889,7 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>46</v>
+        <v>0</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -919,10 +916,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>93</v>
-      </c>
-      <c r="S4">
-        <v>47</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -942,7 +936,7 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -969,10 +963,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>615</v>
-      </c>
-      <c r="S5">
-        <v>315</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -992,7 +983,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1019,9 +1010,6 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="S6">
         <v>0</v>
       </c>
     </row>
@@ -1042,7 +1030,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1069,9 +1057,6 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>1</v>
-      </c>
-      <c r="S7">
         <v>0</v>
       </c>
     </row>
@@ -1092,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>82</v>
+        <v>0</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1119,10 +1104,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>134</v>
-      </c>
-      <c r="S8">
-        <v>52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -1142,7 +1124,7 @@
         <v>0</v>
       </c>
       <c r="H9">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -1169,10 +1151,7 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>13</v>
-      </c>
-      <c r="S9">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -1192,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1219,10 +1198,7 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>17</v>
-      </c>
-      <c r="S10">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -1271,9 +1247,6 @@
       <c r="Q11">
         <v>0</v>
       </c>
-      <c r="S11">
-        <v>0</v>
-      </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C12">
@@ -1321,9 +1294,6 @@
       <c r="Q12">
         <v>0</v>
       </c>
-      <c r="S12">
-        <v>0</v>
-      </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C13">
@@ -1342,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1369,10 +1339,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>44</v>
-      </c>
-      <c r="S13">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -1392,7 +1359,7 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1419,10 +1386,7 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>210</v>
-      </c>
-      <c r="S14">
-        <v>78</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -1471,9 +1435,6 @@
       <c r="Q15">
         <v>0</v>
       </c>
-      <c r="S15">
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C16">
@@ -1521,11 +1482,8 @@
       <c r="Q16">
         <v>0</v>
       </c>
-      <c r="S16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1542,7 +1500,7 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1569,13 +1527,10 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>15</v>
-      </c>
-      <c r="S17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1595,7 +1550,7 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -1622,13 +1577,10 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>31</v>
-      </c>
-      <c r="S18">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1674,11 +1626,8 @@
       <c r="Q19">
         <v>0</v>
       </c>
-      <c r="S19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1695,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -1722,13 +1671,10 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>14</v>
-      </c>
-      <c r="S20">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1748,7 +1694,7 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="I21">
         <v>0</v>
@@ -1775,13 +1721,10 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>62</v>
-      </c>
-      <c r="S21">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1798,7 +1741,7 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -1825,13 +1768,10 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>3</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1848,7 +1788,7 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1875,13 +1815,10 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>2</v>
-      </c>
-      <c r="S23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1898,7 +1835,7 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I24">
         <v>0</v>
@@ -1925,13 +1862,10 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>3</v>
-      </c>
-      <c r="S24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C25">
         <v>25</v>
       </c>
@@ -1977,11 +1911,8 @@
       <c r="Q25">
         <v>0</v>
       </c>
-      <c r="S25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>26</v>
       </c>
@@ -1998,7 +1929,7 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -2025,13 +1956,10 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>4</v>
-      </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C27">
         <v>27</v>
       </c>
@@ -2048,7 +1976,7 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2075,13 +2003,10 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>6</v>
-      </c>
-      <c r="S27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C28">
         <v>28</v>
       </c>
@@ -2098,7 +2023,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -2125,13 +2050,10 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>56</v>
-      </c>
-      <c r="S28">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2148,7 +2070,7 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -2175,13 +2097,10 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>17</v>
-      </c>
-      <c r="S29">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2231,7 +2150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2248,7 +2167,7 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I31">
         <v>0</v>
@@ -2275,10 +2194,10 @@
         <v>0</v>
       </c>
       <c r="Q31">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2342,7 +2261,7 @@
         <v>0</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <v>0</v>
@@ -2369,7 +2288,7 @@
         <v>0</v>
       </c>
       <c r="Q33">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="3:17" x14ac:dyDescent="0.25">
@@ -2389,7 +2308,7 @@
         <v>0</v>
       </c>
       <c r="H34">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -2416,7 +2335,7 @@
         <v>0</v>
       </c>
       <c r="Q34">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="3:17" x14ac:dyDescent="0.25">
@@ -2483,7 +2402,7 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -2510,7 +2429,7 @@
         <v>0</v>
       </c>
       <c r="Q36">
-        <v>28</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="3:17" x14ac:dyDescent="0.25">
@@ -2671,7 +2590,7 @@
         <v>0</v>
       </c>
       <c r="H40">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I40">
         <v>0</v>
@@ -2698,7 +2617,7 @@
         <v>0</v>
       </c>
       <c r="Q40">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="3:17" x14ac:dyDescent="0.25">
@@ -2718,7 +2637,7 @@
         <v>0</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41">
         <v>0</v>
@@ -2745,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="Q41">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="3:17" x14ac:dyDescent="0.25">
@@ -2812,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -2839,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="Q43">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="3:17" x14ac:dyDescent="0.25">
@@ -2953,7 +2872,7 @@
         <v>0</v>
       </c>
       <c r="H46">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I46">
         <v>0</v>
@@ -2980,7 +2899,7 @@
         <v>0</v>
       </c>
       <c r="Q46">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="3:17" x14ac:dyDescent="0.25">
@@ -3000,7 +2919,7 @@
         <v>0</v>
       </c>
       <c r="H47">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I47">
         <v>0</v>
@@ -3027,7 +2946,7 @@
         <v>0</v>
       </c>
       <c r="Q47">
-        <v>12</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="3:17" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
oaks-crisis: Ran Crisis RPA for every month since July 2020
</commit_message>
<xml_diff>
--- a/src/csv/crisis_sfy_2021.xlsx
+++ b/src/csv/crisis_sfy_2021.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23530"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\KHIT\RPA\src\csv\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D238D01D-DC1C-4E74-B885-7EA4E552C4AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="crisis_src" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -297,8 +291,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -361,14 +355,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -415,7 +401,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -447,27 +433,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -499,24 +467,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -692,16 +642,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -775,7 +723,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="C2">
         <v>2</v>
       </c>
@@ -822,7 +770,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="B3" t="s">
         <v>27</v>
       </c>
@@ -833,22 +781,22 @@
         <v>33</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>262</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>268</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>254</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>264</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>264</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>268</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -869,10 +817,10 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="C4">
         <v>4</v>
       </c>
@@ -880,22 +828,22 @@
         <v>34</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>39</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="K4">
         <v>0</v>
@@ -916,10 +864,10 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24">
       <c r="C5">
         <v>5</v>
       </c>
@@ -927,22 +875,22 @@
         <v>35</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>292</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>304</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>293</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>309</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>313</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>315</v>
       </c>
       <c r="K5">
         <v>0</v>
@@ -963,10 +911,10 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1826</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="C6">
         <v>6</v>
       </c>
@@ -983,7 +931,7 @@
         <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I6">
         <v>0</v>
@@ -1010,10 +958,10 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24">
       <c r="C7">
         <v>7</v>
       </c>
@@ -1030,7 +978,7 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1057,10 +1005,10 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="C8">
         <v>8</v>
       </c>
@@ -1074,16 +1022,16 @@
         <v>0</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="J8">
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="K8">
         <v>0</v>
@@ -1104,10 +1052,10 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
       <c r="C9">
         <v>9</v>
       </c>
@@ -1121,16 +1069,16 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K9">
         <v>0</v>
@@ -1151,10 +1099,10 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24">
       <c r="C10">
         <v>10</v>
       </c>
@@ -1168,16 +1116,16 @@
         <v>0</v>
       </c>
       <c r="G10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J10">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K10">
         <v>0</v>
@@ -1198,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24">
       <c r="C11">
         <v>11</v>
       </c>
@@ -1248,7 +1196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="C12">
         <v>12</v>
       </c>
@@ -1295,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="C13">
         <v>13</v>
       </c>
@@ -1309,16 +1257,16 @@
         <v>0</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="H13">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="I13">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="J13">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="K13">
         <v>0</v>
@@ -1339,10 +1287,10 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
       <c r="C14">
         <v>14</v>
       </c>
@@ -1356,16 +1304,16 @@
         <v>0</v>
       </c>
       <c r="G14">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="H14">
-        <v>0</v>
+        <v>84</v>
       </c>
       <c r="I14">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="J14">
-        <v>0</v>
+        <v>78</v>
       </c>
       <c r="K14">
         <v>0</v>
@@ -1386,10 +1334,10 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
       <c r="C15">
         <v>15</v>
       </c>
@@ -1436,7 +1384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="C16">
         <v>16</v>
       </c>
@@ -1483,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="C17">
         <v>17</v>
       </c>
@@ -1494,16 +1442,16 @@
         <v>0</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="G17">
-        <v>0</v>
+        <v>48</v>
       </c>
       <c r="H17">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="I17">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J17">
         <v>0</v>
@@ -1527,10 +1475,10 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="B18" t="s">
         <v>28</v>
       </c>
@@ -1541,22 +1489,22 @@
         <v>48</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G18">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="I18">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1577,10 +1525,10 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="C19">
         <v>19</v>
       </c>
@@ -1588,13 +1536,13 @@
         <v>49</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1624,10 +1572,10 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="C20">
         <v>20</v>
       </c>
@@ -1635,22 +1583,22 @@
         <v>50</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G20">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1671,10 +1619,10 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="B21" t="s">
         <v>29</v>
       </c>
@@ -1685,22 +1633,22 @@
         <v>51</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="I21">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="J21">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="K21">
         <v>0</v>
@@ -1721,10 +1669,10 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="C22">
         <v>22</v>
       </c>
@@ -1747,7 +1695,7 @@
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -1768,10 +1716,10 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="C23">
         <v>23</v>
       </c>
@@ -1791,10 +1739,10 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K23">
         <v>0</v>
@@ -1815,10 +1763,10 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="C24">
         <v>24</v>
       </c>
@@ -1841,7 +1789,7 @@
         <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -1862,10 +1810,10 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="C25">
         <v>25</v>
       </c>
@@ -1912,7 +1860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17">
       <c r="C26">
         <v>26</v>
       </c>
@@ -1932,10 +1880,10 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -1956,10 +1904,10 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="C27">
         <v>27</v>
       </c>
@@ -1967,16 +1915,16 @@
         <v>57</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I27">
         <v>0</v>
@@ -2003,10 +1951,10 @@
         <v>0</v>
       </c>
       <c r="Q27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="C28">
         <v>28</v>
       </c>
@@ -2020,16 +1968,16 @@
         <v>0</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="I28">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="J28">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="K28">
         <v>0</v>
@@ -2050,10 +1998,10 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="C29">
         <v>29</v>
       </c>
@@ -2067,16 +2015,16 @@
         <v>0</v>
       </c>
       <c r="G29">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="H29">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I29">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J29">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="K29">
         <v>0</v>
@@ -2097,10 +2045,10 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -2150,7 +2098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="C31">
         <v>31</v>
       </c>
@@ -2197,7 +2145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="C32">
         <v>32</v>
       </c>
@@ -2244,7 +2192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:17">
       <c r="C33">
         <v>33</v>
       </c>
@@ -2291,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:17">
       <c r="C34">
         <v>34</v>
       </c>
@@ -2338,7 +2286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:17">
       <c r="C35">
         <v>35</v>
       </c>
@@ -2385,7 +2333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:17">
       <c r="C36">
         <v>36</v>
       </c>
@@ -2432,7 +2380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:17">
       <c r="C37">
         <v>37</v>
       </c>
@@ -2479,7 +2427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:17">
       <c r="C38">
         <v>38</v>
       </c>
@@ -2526,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:17">
       <c r="C39">
         <v>39</v>
       </c>
@@ -2573,7 +2521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:17">
       <c r="C40">
         <v>40</v>
       </c>
@@ -2620,7 +2568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:17">
       <c r="C41">
         <v>41</v>
       </c>
@@ -2667,7 +2615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:17">
       <c r="C42">
         <v>42</v>
       </c>
@@ -2714,7 +2662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:17">
       <c r="C43">
         <v>43</v>
       </c>
@@ -2761,7 +2709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:17">
       <c r="C44">
         <v>44</v>
       </c>
@@ -2808,7 +2756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:17">
       <c r="C45">
         <v>45</v>
       </c>
@@ -2855,7 +2803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:17">
       <c r="C46">
         <v>46</v>
       </c>
@@ -2902,7 +2850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:17">
       <c r="C47">
         <v>47</v>
       </c>
@@ -2949,7 +2897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:17">
       <c r="C48">
         <v>48</v>
       </c>
@@ -2996,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
         <v>25</v>
       </c>
@@ -3049,7 +2997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="C50">
         <v>50</v>
       </c>
@@ -3096,7 +3044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="C51">
         <v>51</v>
       </c>
@@ -3143,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:17">
       <c r="C52">
         <v>52</v>
       </c>
@@ -3190,7 +3138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17">
       <c r="C53">
         <v>53</v>
       </c>
@@ -3237,7 +3185,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17">
       <c r="C54">
         <v>54</v>
       </c>
@@ -3284,7 +3232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17">
       <c r="B55" t="s">
         <v>31</v>
       </c>
@@ -3334,7 +3282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17">
       <c r="C56">
         <v>56</v>
       </c>
@@ -3381,7 +3329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17">
       <c r="C57">
         <v>57</v>
       </c>
@@ -3428,7 +3376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17">
       <c r="C58">
         <v>58</v>
       </c>
@@ -3475,7 +3423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17">
       <c r="C59">
         <v>59</v>
       </c>
@@ -3522,7 +3470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17">
       <c r="C60">
         <v>60</v>
       </c>
@@ -3569,7 +3517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17">
       <c r="C61">
         <v>61</v>
       </c>
@@ -3616,7 +3564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17">
       <c r="C62">
         <v>62</v>
       </c>
@@ -3663,7 +3611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17">
       <c r="C63">
         <v>63</v>
       </c>
@@ -3710,7 +3658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17">
       <c r="C64">
         <v>64</v>
       </c>
@@ -3757,7 +3705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22">
       <c r="C65">
         <v>65</v>
       </c>
@@ -3804,7 +3752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22">
       <c r="C66">
         <v>66</v>
       </c>
@@ -3851,7 +3799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22">
       <c r="C67">
         <v>67</v>
       </c>
@@ -3898,7 +3846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22">
       <c r="C68">
         <v>68</v>
       </c>
@@ -3945,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22">
       <c r="C69">
         <v>69</v>
       </c>
@@ -3992,7 +3940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22">
       <c r="C70">
         <v>70</v>
       </c>
@@ -4039,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22">
       <c r="C71">
         <v>71</v>
       </c>
@@ -4086,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22">
       <c r="C72">
         <v>72</v>
       </c>
@@ -4133,7 +4081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22">
       <c r="C73">
         <v>73</v>
       </c>
@@ -4180,7 +4128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22">
       <c r="C74">
         <v>74</v>
       </c>
@@ -4227,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22">
       <c r="A75" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
master (Oaks Crisis): Update scheduling
</commit_message>
<xml_diff>
--- a/src/csv/crisis_sfy_2021.xlsx
+++ b/src/csv/crisis_sfy_2021.xlsx
@@ -799,7 +799,7 @@
         <v>270</v>
       </c>
       <c r="K3">
-        <v>0</v>
+        <v>289</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>1582</v>
+        <v>1871</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -864,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>244</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -893,7 +893,7 @@
         <v>315</v>
       </c>
       <c r="K5">
-        <v>0</v>
+        <v>346</v>
       </c>
       <c r="L5">
         <v>0</v>
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>1826</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -1034,7 +1034,7 @@
         <v>52</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>178</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1081,7 +1081,7 @@
         <v>5</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L9">
         <v>0</v>
@@ -1099,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -1128,7 +1128,7 @@
         <v>7</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="L10">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>28</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -1269,7 +1269,7 @@
         <v>14</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>56</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -1316,7 +1316,7 @@
         <v>78</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>277</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -1507,7 +1507,7 @@
         <v>12</v>
       </c>
       <c r="K18">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>79</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1601,7 +1601,7 @@
         <v>6</v>
       </c>
       <c r="K20">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L20">
         <v>0</v>
@@ -1619,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1651,7 +1651,7 @@
         <v>57</v>
       </c>
       <c r="K21">
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -1669,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>180</v>
+        <v>236</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1698,7 +1698,7 @@
         <v>6</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -1716,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1745,7 +1745,7 @@
         <v>6</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1792,7 +1792,7 @@
         <v>6</v>
       </c>
       <c r="K24">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="L24">
         <v>0</v>
@@ -1810,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1886,7 +1886,7 @@
         <v>6</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L26">
         <v>0</v>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1980,7 +1980,7 @@
         <v>27</v>
       </c>
       <c r="K28">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>98</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2027,7 +2027,7 @@
         <v>33</v>
       </c>
       <c r="K29">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:17">

</xml_diff>

<commit_message>
master: Fix Oaks Crisis typos
</commit_message>
<xml_diff>
--- a/src/csv/crisis_sfy_2021.xlsx
+++ b/src/csv/crisis_sfy_2021.xlsx
@@ -846,7 +846,7 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -1507,7 +1507,7 @@
         <v>12</v>
       </c>
       <c r="K18">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="L18">
         <v>0</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1980,7 +1980,7 @@
         <v>27</v>
       </c>
       <c r="K28">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="L28">
         <v>0</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>124</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2027,7 +2027,7 @@
         <v>33</v>
       </c>
       <c r="K29">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="L29">
         <v>0</v>
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>65</v>
+        <v>78</v>
       </c>
     </row>
     <row r="30" spans="1:17">

</xml_diff>

<commit_message>
master: Fix row 21 in Oaks Crisis
</commit_message>
<xml_diff>
--- a/src/csv/crisis_sfy_2021.xlsx
+++ b/src/csv/crisis_sfy_2021.xlsx
@@ -843,7 +843,7 @@
         <v>49</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="K4">
         <v>57</v>
@@ -864,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>256</v>
+        <v>301</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -1031,10 +1031,10 @@
         <v>50</v>
       </c>
       <c r="J8">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K8">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L8">
         <v>0</v>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1269,7 +1269,7 @@
         <v>14</v>
       </c>
       <c r="K13">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L13">
         <v>0</v>
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -1313,10 +1313,10 @@
         <v>77</v>
       </c>
       <c r="J14">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="K14">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L14">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>360</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -1504,7 +1504,7 @@
         <v>14</v>
       </c>
       <c r="J18">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K18">
         <v>28</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1648,10 +1648,10 @@
         <v>22</v>
       </c>
       <c r="J21">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="K21">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -1669,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>236</v>
+        <v>269</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1977,7 +1977,7 @@
         <v>31</v>
       </c>
       <c r="J28">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="K28">
         <v>13</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2024,7 +2024,7 @@
         <v>6</v>
       </c>
       <c r="J29">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="K29">
         <v>26</v>
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:17">

</xml_diff>

<commit_message>
master: Appleseed RPA maintenance
</commit_message>
<xml_diff>
--- a/src/csv/crisis_sfy_2021.xlsx
+++ b/src/csv/crisis_sfy_2021.xlsx
@@ -802,7 +802,7 @@
         <v>289</v>
       </c>
       <c r="L3">
-        <v>0</v>
+        <v>234</v>
       </c>
       <c r="M3">
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>1871</v>
+        <v>2105</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -849,7 +849,7 @@
         <v>57</v>
       </c>
       <c r="L4">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="M4">
         <v>0</v>
@@ -864,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>301</v>
+        <v>365</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -896,7 +896,7 @@
         <v>346</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>298</v>
       </c>
       <c r="M5">
         <v>0</v>
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>2172</v>
+        <v>2470</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -990,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
         <v>0</v>
@@ -1005,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:24">
@@ -1037,7 +1037,7 @@
         <v>40</v>
       </c>
       <c r="L8">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="M8">
         <v>0</v>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>216</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1084,7 +1084,7 @@
         <v>3</v>
       </c>
       <c r="L9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M9">
         <v>0</v>
@@ -1099,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -1131,7 +1131,7 @@
         <v>12</v>
       </c>
       <c r="L10">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M10">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>40</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -1272,7 +1272,7 @@
         <v>26</v>
       </c>
       <c r="L13">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M13">
         <v>0</v>
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>82</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -1319,7 +1319,7 @@
         <v>81</v>
       </c>
       <c r="L14">
-        <v>0</v>
+        <v>119</v>
       </c>
       <c r="M14">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>356</v>
+        <v>475</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -1510,7 +1510,7 @@
         <v>28</v>
       </c>
       <c r="L18">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="M18">
         <v>0</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>110</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1557,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="M19">
         <v>0</v>
@@ -1572,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1604,7 +1604,7 @@
         <v>10</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M20">
         <v>0</v>
@@ -1619,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1654,7 +1654,7 @@
         <v>72</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="M21">
         <v>0</v>
@@ -1669,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>269</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1701,7 +1701,7 @@
         <v>4</v>
       </c>
       <c r="L22">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="M22">
         <v>0</v>
@@ -1716,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1795,7 +1795,7 @@
         <v>6</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="M24">
         <v>0</v>
@@ -1810,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1842,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M25">
         <v>0</v>
@@ -1857,7 +1857,7 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1889,7 +1889,7 @@
         <v>5</v>
       </c>
       <c r="L26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M26">
         <v>0</v>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1983,7 +1983,7 @@
         <v>13</v>
       </c>
       <c r="L28">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="M28">
         <v>0</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2030,7 +2030,7 @@
         <v>26</v>
       </c>
       <c r="L29">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="M29">
         <v>0</v>
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>72</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="1:17">

</xml_diff>

<commit_message>
master: general maintenance updates
</commit_message>
<xml_diff>
--- a/src/csv/crisis_sfy_2021.xlsx
+++ b/src/csv/crisis_sfy_2021.xlsx
@@ -805,7 +805,7 @@
         <v>234</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>286</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>2105</v>
+        <v>2391</v>
       </c>
     </row>
     <row r="4" spans="1:24">
@@ -852,7 +852,7 @@
         <v>64</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -864,7 +864,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>365</v>
+        <v>445</v>
       </c>
     </row>
     <row r="5" spans="1:24">
@@ -899,7 +899,7 @@
         <v>298</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>366</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -911,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="Q5">
-        <v>2470</v>
+        <v>2836</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -1040,7 +1040,7 @@
         <v>65</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="N8">
         <v>0</v>
@@ -1052,7 +1052,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>281</v>
+        <v>334</v>
       </c>
     </row>
     <row r="9" spans="1:24">
@@ -1087,7 +1087,7 @@
         <v>8</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="N9">
         <v>0</v>
@@ -1099,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:24">
@@ -1134,7 +1134,7 @@
         <v>15</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="N10">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:24">
@@ -1275,7 +1275,7 @@
         <v>30</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="N13">
         <v>0</v>
@@ -1287,7 +1287,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>112</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:24">
@@ -1322,7 +1322,7 @@
         <v>119</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="N14">
         <v>0</v>
@@ -1334,7 +1334,7 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>475</v>
+        <v>571</v>
       </c>
     </row>
     <row r="15" spans="1:24">
@@ -1513,7 +1513,7 @@
         <v>22</v>
       </c>
       <c r="M18">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="N18">
         <v>0</v>
@@ -1525,7 +1525,7 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>132</v>
+        <v>169</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1607,7 +1607,7 @@
         <v>3</v>
       </c>
       <c r="M20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N20">
         <v>0</v>
@@ -1619,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="Q20">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1657,7 +1657,7 @@
         <v>67</v>
       </c>
       <c r="M21">
-        <v>0</v>
+        <v>75</v>
       </c>
       <c r="N21">
         <v>0</v>
@@ -1669,7 +1669,7 @@
         <v>0</v>
       </c>
       <c r="Q21">
-        <v>336</v>
+        <v>411</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1704,7 +1704,7 @@
         <v>3</v>
       </c>
       <c r="M22">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="N22">
         <v>0</v>
@@ -1716,7 +1716,7 @@
         <v>0</v>
       </c>
       <c r="Q22">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1751,7 +1751,7 @@
         <v>0</v>
       </c>
       <c r="M23">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N23">
         <v>0</v>
@@ -1763,7 +1763,7 @@
         <v>0</v>
       </c>
       <c r="Q23">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1798,7 +1798,7 @@
         <v>4</v>
       </c>
       <c r="M24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="N24">
         <v>0</v>
@@ -1810,7 +1810,7 @@
         <v>0</v>
       </c>
       <c r="Q24">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1845,7 +1845,7 @@
         <v>1</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25">
         <v>0</v>
@@ -1857,7 +1857,7 @@
         <v>0</v>
       </c>
       <c r="Q25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1892,7 +1892,7 @@
         <v>2</v>
       </c>
       <c r="M26">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="N26">
         <v>0</v>
@@ -1904,7 +1904,7 @@
         <v>0</v>
       </c>
       <c r="Q26">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1986,7 +1986,7 @@
         <v>8</v>
       </c>
       <c r="M28">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="N28">
         <v>0</v>
@@ -1998,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="Q28">
-        <v>103</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -2033,7 +2033,7 @@
         <v>12</v>
       </c>
       <c r="M29">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="N29">
         <v>0</v>
@@ -2045,7 +2045,7 @@
         <v>0</v>
       </c>
       <c r="Q29">
-        <v>84</v>
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:17">

</xml_diff>